<commit_message>
update the migration script
add rbac related data
</commit_message>
<xml_diff>
--- a/docs/roles.xlsx
+++ b/docs/roles.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
   <si>
     <t>程序员</t>
   </si>
@@ -56,12 +56,6 @@
     <t>创建</t>
   </si>
   <si>
-    <t>保存</t>
-  </si>
-  <si>
-    <t>查看</t>
-  </si>
-  <si>
     <t>导出</t>
   </si>
   <si>
@@ -102,6 +96,9 @@
   </si>
   <si>
     <t>*- 表示有此权限，但是仅限自己创建的</t>
+  </si>
+  <si>
+    <t>列表查看</t>
   </si>
 </sst>
 </file>
@@ -163,7 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -176,6 +173,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -485,7 +485,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -497,10 +497,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -513,188 +513,186 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
+      <c r="A7" s="7"/>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>14</v>
+      <c r="A11" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -703,61 +701,61 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A14"/>
     <mergeCell ref="A15:A17"/>
   </mergeCells>

</xml_diff>